<commit_message>
Corrected position of R4
</commit_message>
<xml_diff>
--- a/gerber files/AEMSUCA-R3-coordinates.xlsx
+++ b/gerber files/AEMSUCA-R3-coordinates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrsik\Documents\AEMSUCA\gerber files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\AEM boards\AEMSUCA\eagle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B230CDA-9C22-482C-B2FC-A87347AE966E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC49146-5D9D-4E44-99D6-4B1630D7740C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BE642D02-475E-4F28-AFF5-4B57E895980E}"/>
   </bookViews>
@@ -476,7 +476,7 @@
   <dimension ref="A1:F180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -740,7 +740,7 @@
         <v>15.4</v>
       </c>
       <c r="D13" s="4">
-        <v>2.9</v>
+        <v>4.7</v>
       </c>
       <c r="E13" t="s">
         <v>0</v>

</xml_diff>